<commit_message>
Backend implementation is done.
</commit_message>
<xml_diff>
--- a/documents/API_Doc.xlsx
+++ b/documents/API_Doc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kotresh\Desktop\InternCraft\BDFL-Tech\hiring-tracker\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6003A1CA-39E7-467B-A036-870E44FDD030}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF2D5697-7005-4CD4-B3BA-CD37B4FE7768}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -94,8 +94,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -123,8 +131,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,8 +416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -416,28 +425,28 @@
     <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="49.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="81" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
@@ -503,5 +512,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
4 API templates with data.json
</commit_message>
<xml_diff>
--- a/documents/API_Doc.xlsx
+++ b/documents/API_Doc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kotresh\Desktop\InternCraft\BDFL-Tech\hiring-tracker\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF2D5697-7005-4CD4-B3BA-CD37B4FE7768}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01FE4DD0-ED6E-42A2-AF70-ADCEFF9C94A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -416,8 +416,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="A4:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
API sample integration code is implemented updating the backend with PUT request and CORS provision.
</commit_message>
<xml_diff>
--- a/documents/API_Doc.xlsx
+++ b/documents/API_Doc.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kotresh\Desktop\InternCraft\BDFL-Tech\hiring-tracker\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01FE4DD0-ED6E-42A2-AF70-ADCEFF9C94A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FCFA6E4-A824-4954-ADA0-1124A2E78BB2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t>Page</t>
   </si>
@@ -88,6 +88,18 @@
   </si>
   <si>
     <t>{ requestId : 1 } // optional</t>
+  </si>
+  <si>
+    <t>Login Page</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>/api/authenticate</t>
+  </si>
+  <si>
+    <t>{ username: "admin", password: "admin@internship" }</t>
   </si>
 </sst>
 </file>
@@ -414,10 +426,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="A4:F4"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,6 +522,26 @@
         <v>15</v>
       </c>
     </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>